<commit_message>
sheet name update in excel
</commit_message>
<xml_diff>
--- a/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
+++ b/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId1" sheetId="1" name="Add a Loanbook data"/>
     <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
     <sheet r:id="rId3" sheetId="3" name="Sheet3"/>
   </sheets>
@@ -72,7 +72,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -466,7 +466,7 @@
     <col min="7" max="7" style="10" width="27.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="159">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="186.75">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -512,7 +512,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -523,7 +523,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -534,7 +534,7 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -545,7 +545,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>

</xml_diff>

<commit_message>
add a loanbook form test method update
</commit_message>
<xml_diff>
--- a/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
+++ b/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -51,7 +51,26 @@
     <t>Astute Financial Management</t>
   </si>
   <si>
+    <t>Operating since 2000, Astute has established itself as a highly respected financial services provider with a membership base comprising of approximately 500 finance, insurance and financial planning specialists across Australia.
+We are a privately owned business, leading the market with a fully integrated financial services offering to our members. With a loan book of over $20 billion dollars, we are well positioned for growth.</t>
+  </si>
+  <si>
+    <t>Toowong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000000                                                                                                                              </t>
+  </si>
+  <si>
     <t>Aussie</t>
+  </si>
+  <si>
+    <t>Aussie works closely with industry and government to ensure a strong customer first industry. Our team are passionate about continuing to find ways to improve the home loan experience. We’ll give you the confidence to make a move.</t>
+  </si>
+  <si>
+    <t>philippines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2100000                                                                                                                              </t>
   </si>
   <si>
     <t>PLAN Australia</t>
@@ -516,27 +535,51 @@
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6">
+        <v>27.4843</v>
+      </c>
+      <c r="E3" s="6">
+        <v>152.9837</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6">
+        <v>12.8797</v>
+      </c>
+      <c r="E4" s="6">
+        <v>121.774</v>
+      </c>
+      <c r="F4" s="7">
+        <v>135000</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>

</xml_diff>

<commit_message>
excel sheet row delete
</commit_message>
<xml_diff>
--- a/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
+++ b/loanbookforsale/src/main/java/loanbookforsale/qa/testdata/loanbookforsale.xlsx
@@ -470,7 +470,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -531,7 +531,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="48">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -587,15 +587,6 @@
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="21">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>